<commit_message>
Completed adding excel MCVanillaChoice option
</commit_message>
<xml_diff>
--- a/JoshiProject1.xlsx
+++ b/JoshiProject1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Spot</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t>BSPrice</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>straddle</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
+  <si>
+    <t>expiry</t>
+  </si>
+  <si>
+    <t>option name</t>
+  </si>
+  <si>
+    <t>num Paths</t>
   </si>
 </sst>
 </file>
@@ -172,7 +199,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1091772278879601"/>
+          <c:x val="0.10917722788796011"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1542,11 +1569,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53856128"/>
+        <c:axId val="54904704"/>
         <c:axId val="55050624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53856128"/>
+        <c:axId val="54904704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,7 +1629,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53856128"/>
+        <c:crossAx val="54904704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1614,7 +1641,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1630,8 +1657,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26891632006966304"/>
-          <c:y val="2.8275009877756649E-2"/>
+          <c:x val="0.26891632006966315"/>
+          <c:y val="2.8275009877756652E-2"/>
           <c:w val="0.6738373047041657"/>
           <c:h val="0.8971166436276885"/>
         </c:manualLayout>
@@ -2994,7 +3021,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3032,8 +3059,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10951222115528771"/>
-          <c:y val="6.4986002424438577E-3"/>
+          <c:x val="0.10951222115528773"/>
+          <c:y val="6.4986002424438595E-3"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -3045,7 +3072,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.4488407699037621E-2"/>
           <c:y val="0.19461706996942271"/>
-          <c:w val="0.85871446655282824"/>
+          <c:w val="0.85871446655282835"/>
           <c:h val="0.63890604507981763"/>
         </c:manualLayout>
       </c:layout>
@@ -3387,7 +3414,7 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:axId val="55106176"/>
-        <c:axId val="55452032"/>
+        <c:axId val="57282944"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="55106176"/>
@@ -3397,12 +3424,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55452032"/>
+        <c:crossAx val="57282944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55452032"/>
+        <c:axId val="57282944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3419,7 +3446,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3773,23 +3800,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="55459200"/>
-        <c:axId val="55481472"/>
+        <c:axId val="57290112"/>
+        <c:axId val="57316480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55459200"/>
+        <c:axId val="57290112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55481472"/>
+        <c:crossAx val="57316480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55481472"/>
+        <c:axId val="57316480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3797,7 +3824,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55459200"/>
+        <c:crossAx val="57290112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3809,7 +3836,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4110,11 +4137,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="55505664"/>
-        <c:axId val="55507584"/>
+        <c:axId val="57475840"/>
+        <c:axId val="57477760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55505664"/>
+        <c:axId val="57475840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4123,12 +4150,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55507584"/>
+        <c:crossAx val="57477760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55507584"/>
+        <c:axId val="57477760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4138,7 +4165,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55505664"/>
+        <c:crossAx val="57475840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4147,7 +4174,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4593,10 +4620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S361"/>
+  <dimension ref="A1:S364"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B357" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G361" sqref="G361"/>
+      <selection activeCell="I365" sqref="I365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17844,6 +17871,32 @@
         <v>8.5916594188251452</v>
       </c>
     </row>
+    <row r="360" spans="2:11">
+      <c r="B360" t="s">
+        <v>0</v>
+      </c>
+      <c r="C360" t="s">
+        <v>28</v>
+      </c>
+      <c r="D360" t="s">
+        <v>29</v>
+      </c>
+      <c r="E360" t="s">
+        <v>30</v>
+      </c>
+      <c r="F360" t="s">
+        <v>31</v>
+      </c>
+      <c r="G360" t="s">
+        <v>32</v>
+      </c>
+      <c r="H360" t="s">
+        <v>33</v>
+      </c>
+      <c r="I360" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="361" spans="2:11">
       <c r="B361">
         <v>100</v>
@@ -17860,18 +17913,111 @@
       <c r="F361">
         <v>1</v>
       </c>
-      <c r="G361">
-        <v>0</v>
+      <c r="G361" t="s">
+        <v>25</v>
       </c>
       <c r="H361">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="I361">
         <v>100</v>
       </c>
       <c r="J361">
         <f>MCVanillaChoice(B361:I361)</f>
-        <v>3.7036750015272091</v>
+        <v>3.7097594233854667</v>
+      </c>
+      <c r="K361" t="str">
+        <f>MCVanillaChoice()</f>
+        <v>non number cell asked to be a number</v>
+      </c>
+    </row>
+    <row r="362" spans="2:11">
+      <c r="B362">
+        <v>100</v>
+      </c>
+      <c r="C362">
+        <v>0.05</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>0.15</v>
+      </c>
+      <c r="F362">
+        <v>1</v>
+      </c>
+      <c r="G362" t="s">
+        <v>26</v>
+      </c>
+      <c r="H362">
+        <v>100000</v>
+      </c>
+      <c r="I362">
+        <v>100</v>
+      </c>
+      <c r="J362">
+        <f>MCVanillaChoice(B362:I362)</f>
+        <v>8.5922250878491866</v>
+      </c>
+    </row>
+    <row r="363" spans="2:11">
+      <c r="B363">
+        <v>100</v>
+      </c>
+      <c r="C363">
+        <v>0.05</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>0.15</v>
+      </c>
+      <c r="F363">
+        <v>1</v>
+      </c>
+      <c r="G363" t="s">
+        <v>27</v>
+      </c>
+      <c r="H363">
+        <v>100000</v>
+      </c>
+      <c r="I363">
+        <v>100</v>
+      </c>
+      <c r="J363">
+        <f>MCVanillaChoice(B363:I363)</f>
+        <v>12.301984511234695</v>
+      </c>
+    </row>
+    <row r="364" spans="2:11">
+      <c r="B364">
+        <v>100</v>
+      </c>
+      <c r="C364">
+        <v>0.05</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>0.15</v>
+      </c>
+      <c r="F364">
+        <v>1</v>
+      </c>
+      <c r="G364" t="s">
+        <v>27</v>
+      </c>
+      <c r="H364">
+        <v>100000</v>
+      </c>
+      <c r="I364">
+        <v>90</v>
+      </c>
+      <c r="J364">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ThursEvening Office going home
</commit_message>
<xml_diff>
--- a/JoshiProject1.xlsx
+++ b/JoshiProject1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="15255" windowHeight="7170"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15255" windowHeight="6240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Spot</t>
   </si>
@@ -1575,11 +1575,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="55953280"/>
-        <c:axId val="57147776"/>
+        <c:axId val="53541120"/>
+        <c:axId val="54735616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55953280"/>
+        <c:axId val="53541120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,12 +1604,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57147776"/>
+        <c:crossAx val="54735616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57147776"/>
+        <c:axId val="54735616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,7 +1635,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55953280"/>
+        <c:crossAx val="53541120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1647,7 +1647,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1663,7 +1663,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26891632006966343"/>
+          <c:x val="0.26891632006966404"/>
           <c:y val="2.8275009877756652E-2"/>
           <c:w val="0.6738373047041657"/>
           <c:h val="0.8971166436276885"/>
@@ -2991,23 +2991,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57186176"/>
-        <c:axId val="57187712"/>
+        <c:axId val="54757632"/>
+        <c:axId val="54767616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57186176"/>
+        <c:axId val="54757632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57187712"/>
+        <c:crossAx val="54767616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57187712"/>
+        <c:axId val="54767616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3015,7 +3015,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57186176"/>
+        <c:crossAx val="54757632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3027,7 +3027,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3065,8 +3065,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1095122211552878"/>
-          <c:y val="6.4986002424438647E-3"/>
+          <c:x val="0.10951222115528797"/>
+          <c:y val="6.4986002424438777E-3"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -3078,7 +3078,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.4488407699037621E-2"/>
           <c:y val="0.19461706996942271"/>
-          <c:w val="0.85871446655282879"/>
+          <c:w val="0.85871446655282946"/>
           <c:h val="0.63890604507981763"/>
         </c:manualLayout>
       </c:layout>
@@ -3419,23 +3419,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57203328"/>
-        <c:axId val="57282944"/>
+        <c:axId val="54774784"/>
+        <c:axId val="57479936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57203328"/>
+        <c:axId val="54774784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57282944"/>
+        <c:crossAx val="57479936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57282944"/>
+        <c:axId val="57479936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3443,7 +3443,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57203328"/>
+        <c:crossAx val="54774784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3452,7 +3452,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3806,23 +3806,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57290112"/>
-        <c:axId val="57320576"/>
+        <c:axId val="57516032"/>
+        <c:axId val="57517568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57290112"/>
+        <c:axId val="57516032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57320576"/>
+        <c:crossAx val="57517568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57320576"/>
+        <c:axId val="57517568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3830,7 +3830,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57290112"/>
+        <c:crossAx val="57516032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3842,7 +3842,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4143,11 +4143,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58786560"/>
-        <c:axId val="58788480"/>
+        <c:axId val="57533568"/>
+        <c:axId val="57535488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58786560"/>
+        <c:axId val="57533568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4156,12 +4156,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58788480"/>
+        <c:crossAx val="57535488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58788480"/>
+        <c:axId val="57535488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4171,7 +4171,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58786560"/>
+        <c:crossAx val="57533568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4180,7 +4180,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4626,15 +4626,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S365"/>
+  <dimension ref="A1:S367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B357" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J363" sqref="J363"/>
+    <sheetView tabSelected="1" topLeftCell="B345" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J368" sqref="J368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" customWidth="1"/>
     <col min="18" max="18" width="8.140625" customWidth="1"/>
     <col min="19" max="19" width="11.42578125" customWidth="1"/>
@@ -18054,6 +18054,66 @@
       <c r="J365">
         <f>MCVanillaChoice(B365:I365)</f>
         <v>4.8824656644637052</v>
+      </c>
+    </row>
+    <row r="366" spans="2:11">
+      <c r="B366">
+        <v>100</v>
+      </c>
+      <c r="C366">
+        <v>0.05</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>0.15</v>
+      </c>
+      <c r="F366">
+        <v>1</v>
+      </c>
+      <c r="G366" t="s">
+        <v>35</v>
+      </c>
+      <c r="H366">
+        <v>10000</v>
+      </c>
+      <c r="I366">
+        <v>100</v>
+      </c>
+      <c r="J366">
+        <f>MCVanillaChoice(B366:I366)</f>
+        <v>5.0150582795687368</v>
+      </c>
+    </row>
+    <row r="367" spans="2:11">
+      <c r="B367">
+        <v>100</v>
+      </c>
+      <c r="C367">
+        <v>0.05</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>0.15</v>
+      </c>
+      <c r="F367">
+        <v>1</v>
+      </c>
+      <c r="G367" t="s">
+        <v>25</v>
+      </c>
+      <c r="H367">
+        <v>100000</v>
+      </c>
+      <c r="I367">
+        <v>100</v>
+      </c>
+      <c r="J367">
+        <f>MCVanillaChoice(B367:I367)</f>
+        <v>3.7097594233854667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>